<commit_message>
Finish the alpha 1.0 Search from database
</commit_message>
<xml_diff>
--- a/XSheet/DOC/XSheetFC流程.xlsx
+++ b/XSheet/DOC/XSheetFC流程.xlsx
@@ -9,22 +9,23 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="10815" windowHeight="5175" firstSheet="7" activeTab="10"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="10815" windowHeight="5175" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Config" sheetId="2" r:id="rId2"/>
     <sheet name="总流程" sheetId="5" r:id="rId3"/>
-    <sheet name="根据Config配置--Sheet切换" sheetId="6" r:id="rId4"/>
-    <sheet name="根据Config配置--单元格选择" sheetId="8" r:id="rId5"/>
-    <sheet name="根据Config配置--回车事件" sheetId="10" r:id="rId6"/>
-    <sheet name="SQLAction_Search" sheetId="13" r:id="rId7"/>
-    <sheet name="SQLAction_CUD" sheetId="14" r:id="rId8"/>
-    <sheet name="Main与PopUp交互" sheetId="16" r:id="rId9"/>
-    <sheet name="Execute流程" sheetId="17" r:id="rId10"/>
-    <sheet name="类设计" sheetId="11" r:id="rId11"/>
-    <sheet name="事件绑定流程" sheetId="12" r:id="rId12"/>
-    <sheet name="使用模式" sheetId="18" r:id="rId13"/>
+    <sheet name="XSheet初始化" sheetId="19" r:id="rId4"/>
+    <sheet name="根据Config配置--Sheet切换" sheetId="6" r:id="rId5"/>
+    <sheet name="根据Config配置--单元格选择" sheetId="8" r:id="rId6"/>
+    <sheet name="根据Config配置--回车事件" sheetId="10" r:id="rId7"/>
+    <sheet name="SQLAction_Search" sheetId="13" r:id="rId8"/>
+    <sheet name="SQLAction_CUD" sheetId="14" r:id="rId9"/>
+    <sheet name="Main与PopUp交互" sheetId="16" r:id="rId10"/>
+    <sheet name="Execute流程" sheetId="17" r:id="rId11"/>
+    <sheet name="类设计" sheetId="11" r:id="rId12"/>
+    <sheet name="事件绑定流程" sheetId="12" r:id="rId13"/>
+    <sheet name="使用模式" sheetId="18" r:id="rId14"/>
   </sheets>
   <definedNames>
     <definedName name="test">类设计!$H$21:$K$27</definedName>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="22">
   <si>
     <t>发票号：</t>
   </si>
@@ -109,6 +110,10 @@
   </si>
   <si>
     <t>1.鼠标选中表格，点击Search按钮，获取查询数据</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -976,7 +981,1054 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="矩形 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3514725" y="342899"/>
+          <a:ext cx="1190625" cy="447675"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>事件执行</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="矩形 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3514725" y="1000124"/>
+          <a:ext cx="1190625" cy="447675"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>读取事件所属</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>Command</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="矩形 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3514725" y="1628774"/>
+          <a:ext cx="1190625" cy="447675"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>循环，依次选取</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>action</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="矩形 4"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3514725" y="2352674"/>
+          <a:ext cx="1190625" cy="447675"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>判断</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>Action</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>动作</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>681038</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>681038</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="直接箭头连接符 6"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="2" idx="2"/>
+          <a:endCxn id="3" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4110038" y="790574"/>
+          <a:ext cx="0" cy="209550"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>681038</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>681038</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="直接箭头连接符 8"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="3" idx="2"/>
+          <a:endCxn id="4" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4110038" y="1447799"/>
+          <a:ext cx="0" cy="180975"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>681038</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>681038</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="直接箭头连接符 9"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="4" idx="2"/>
+          <a:endCxn id="5" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4110038" y="2076449"/>
+          <a:ext cx="0" cy="276225"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="矩形 16"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3514725" y="3076574"/>
+          <a:ext cx="1190625" cy="447675"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>执行</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>Action</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>对象对应的动作</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>681038</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>681038</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="直接箭头连接符 18"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="5" idx="2"/>
+          <a:endCxn id="17" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4110038" y="2800349"/>
+          <a:ext cx="0" cy="276225"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="矩形 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3105150" y="342900"/>
+          <a:ext cx="1352550" cy="619125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>读取全部</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>Config</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>配置信息</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="矩形 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3105150" y="1181100"/>
+          <a:ext cx="1352550" cy="619125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>将</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>App</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>信息显示在状态栏中</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>123826</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="矩形 4"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3086100" y="2028825"/>
+          <a:ext cx="1838326" cy="704850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>初始化全部</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>Sheet</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>，依次存入</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>App</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>中</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="zh-CN" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>以及</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Dictionary&lt;String,Sheet&gt;</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="zh-CN">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>419099</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>238124</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="矩形 5"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1790699" y="2914650"/>
+          <a:ext cx="1876425" cy="771525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>初始化全部</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>Command</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>，依次存入</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>Sheet</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>中以及</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>Dictionary&lt;String,Command&gt;</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="矩形 6"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1704975" y="3838575"/>
+          <a:ext cx="1924050" cy="752475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>初始化全部</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>Action</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>，依次存入</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>Command</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>中</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="zh-CN" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>以及</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Dictionary&lt;String,Action&gt;</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>581024</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="矩形 7"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4010024" y="2962275"/>
+          <a:ext cx="2247901" cy="771525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>初始化全部</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>DefinedName</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>，依次存入</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>Sheet</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>的</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>Table</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>以及</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>Range</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>中以及</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>Dictionary&lt;String,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>DefinedName</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>&gt;</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -3695,7 +4747,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -6309,7 +7361,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -8633,7 +9685,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -10843,7 +11895,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -12442,7 +13494,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -12827,7 +13879,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -14597,512 +15649,6 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>171449</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>104774</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="矩形 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3514725" y="342899"/>
-          <a:ext cx="1190625" cy="447675"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
-            <a:t>事件执行</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>142874</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>76199</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="矩形 2"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3514725" y="1000124"/>
-          <a:ext cx="1190625" cy="447675"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
-            <a:t>读取事件所属</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
-            <a:t>Command</a:t>
-          </a:r>
-          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>85724</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>19049</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="矩形 3"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3514725" y="1628774"/>
-          <a:ext cx="1190625" cy="447675"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
-            <a:t>循环，依次选取</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
-            <a:t>action</a:t>
-          </a:r>
-          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>123824</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>57149</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="矩形 4"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3514725" y="2352674"/>
-          <a:ext cx="1190625" cy="447675"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
-            <a:t>判断</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
-            <a:t>Action</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
-            <a:t>动作</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>681038</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>104774</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>681038</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>142874</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="7" name="直接箭头连接符 6"/>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="2" idx="2"/>
-          <a:endCxn id="3" idx="0"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4110038" y="790574"/>
-          <a:ext cx="0" cy="209550"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>681038</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>76199</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>681038</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>85724</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="9" name="直接箭头连接符 8"/>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="3" idx="2"/>
-          <a:endCxn id="4" idx="0"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4110038" y="1447799"/>
-          <a:ext cx="0" cy="180975"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>681038</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>19049</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>681038</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>123824</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="10" name="直接箭头连接符 9"/>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="4" idx="2"/>
-          <a:endCxn id="5" idx="0"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4110038" y="2076449"/>
-          <a:ext cx="0" cy="276225"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>161924</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>95249</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="17" name="矩形 16"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3514725" y="3076574"/>
-          <a:ext cx="1190625" cy="447675"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
-            <a:t>执行</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
-            <a:t>Action</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
-            <a:t>对象对应的动作</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>681038</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>57149</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>681038</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>161924</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="19" name="直接箭头连接符 18"/>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="5" idx="2"/>
-          <a:endCxn id="17" idx="0"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4110038" y="2800349"/>
-          <a:ext cx="0" cy="276225"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -15405,9 +15951,9 @@
   <a:objectDefaults>
     <a:spDef>
       <a:spPr/>
-      <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+      <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
       <a:lstStyle>
-        <a:defPPr algn="l">
+        <a:defPPr algn="ctr">
           <a:defRPr sz="1100"/>
         </a:defPPr>
       </a:lstStyle>
@@ -15949,6 +16495,22 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
@@ -15960,12 +16522,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="AK3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView topLeftCell="G7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="V32" sqref="V32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -15982,7 +16544,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -15998,7 +16560,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3"/>
   <sheetViews>
@@ -16065,9 +16627,31 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="J28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="28" spans="10:10" x14ac:dyDescent="0.15">
+      <c r="J28" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:AH16"/>
   <sheetViews>
-    <sheetView topLeftCell="D7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="K47" sqref="K47"/>
     </sheetView>
   </sheetViews>
@@ -16136,7 +16720,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:AH27"/>
   <sheetViews>
@@ -16212,7 +16796,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:AH16"/>
   <sheetViews>
@@ -16285,7 +16869,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -16301,7 +16885,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="T10"/>
   <sheetViews>
@@ -16321,20 +16905,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <sheetData/>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>